<commit_message>
test1_rembg output + time test2_image output + time
</commit_message>
<xml_diff>
--- a/test/image-background-remove-tool/time_order.xlsx
+++ b/test/image-background-remove-tool/time_order.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="105">
   <si>
     <t>序号</t>
   </si>
@@ -28,73 +28,70 @@
     <t>处理时间</t>
   </si>
   <si>
-    <t>O1CN01Hin2DC1ctryEH0Vpz_!!167873659</t>
-  </si>
-  <si>
-    <t>jpg_430x430q90.jpg</t>
-  </si>
-  <si>
-    <t>12.741390705108643 s</t>
+    <t>O1CN01Hin2DC1ctryEH0Vpz_!!167873659.jpg_430x430q90</t>
+  </si>
+  <si>
+    <t>jpg</t>
+  </si>
+  <si>
+    <t>12.01 s</t>
   </si>
   <si>
     <t>D-CONVERSE-06-16-22-GBL-HP-P2-SUMMER-HEAT-RUN-STAR-MOTION-2</t>
   </si>
   <si>
-    <t>jpg</t>
-  </si>
-  <si>
-    <t>48.05078983306885 s</t>
+    <t>42.56 s</t>
   </si>
   <si>
     <t>02-927</t>
   </si>
   <si>
-    <t>12.63382601737976 s</t>
-  </si>
-  <si>
-    <t>O1CN01dyYJxH1oPtOYNu0Vv_!!3108485218</t>
-  </si>
-  <si>
-    <t>8.878468036651611 s</t>
+    <t>11.90 s</t>
+  </si>
+  <si>
+    <t>O1CN01dyYJxH1oPtOYNu0Vv_!!3108485218.jpg_430x430q90</t>
+  </si>
+  <si>
+    <t>7.89 s</t>
   </si>
   <si>
     <t>O1CN01YcUA682J5yIP6tvig_!!2213974649371</t>
   </si>
   <si>
-    <t>25.424052000045776 s</t>
+    <t>19.73 s</t>
   </si>
   <si>
     <t>O1CN01bdJE111bfpy1W9I0G_!!876583493</t>
   </si>
   <si>
-    <t>45.00161004066467 s</t>
-  </si>
-  <si>
-    <t>628807b266ce49</t>
-  </si>
-  <si>
-    <t>95829316.png</t>
-  </si>
-  <si>
-    <t>9.553396940231323 s</t>
-  </si>
-  <si>
-    <t>O1CN01AhUfEa2CKRUecpgLN_!!92688455</t>
-  </si>
-  <si>
-    <t>9.330546855926514 s</t>
-  </si>
-  <si>
-    <t>O1CN015QDtQa285Y47ycvCE_!!3605347881</t>
-  </si>
-  <si>
-    <t>8.902204751968384 s</t>
+    <t>35.09 s</t>
+  </si>
+  <si>
+    <t>628807b266ce49.95829316</t>
+  </si>
+  <si>
+    <t>png</t>
+  </si>
+  <si>
+    <t>9.43 s</t>
+  </si>
+  <si>
+    <t>O1CN01AhUfEa2CKRUecpgLN_!!92688455.jpg_430x430q90</t>
+  </si>
+  <si>
+    <t>8.97 s</t>
+  </si>
+  <si>
+    <t>O1CN015QDtQa285Y47ycvCE_!!3605347881.jpg_430x430q90</t>
+  </si>
+  <si>
+    <t>8.07 s</t>
   </si>
   <si>
     <t>O1CN01nfxN9C1xh8qpUAOsN_!!2259016474</t>
   </si>
   <si>
-    <t>22.813779830932617 s</t>
+    <t>23.81 s</t>
   </si>
   <si>
     <t>98150-22VX_F</t>
@@ -103,238 +100,235 @@
     <t>webp</t>
   </si>
   <si>
-    <t>16.21798014640808 s</t>
+    <t>24.09 s</t>
   </si>
   <si>
     <t>eb8f4c4e-1ada-4c9e-a95a-f182031cfb51</t>
   </si>
   <si>
-    <t>110.85805177688599 s</t>
+    <t>115.06 s</t>
   </si>
   <si>
     <t>O1CN01nzgzZG1oPtJXjAGEp_!!3108485218</t>
   </si>
   <si>
-    <t>27.91781497001648 s</t>
+    <t>30.56 s</t>
   </si>
   <si>
     <t>f915cc20-f3c6-426e-8e47-4577190f7d83</t>
   </si>
   <si>
-    <t>28.01368999481201 s</t>
+    <t>31.58 s</t>
   </si>
   <si>
     <t>xeric-leadfoot-automatic-gunmetal-orange-2_800c2aea-167a-4b96-97bf-8556736c2c3b_720x</t>
   </si>
   <si>
-    <t>18.40589213371277 s</t>
+    <t>24.07 s</t>
   </si>
   <si>
     <t>ed0e6efb-0e43-474d-a09c-0a270a9c00f5</t>
   </si>
   <si>
-    <t>21.318711042404175 s</t>
+    <t>25.85 s</t>
   </si>
   <si>
     <t>homepage-opternative-grid</t>
   </si>
   <si>
-    <t>10.689327239990234 s</t>
-  </si>
-  <si>
-    <t>O1CN01NVlKjz1GaFOADKpmu_!!738840638-0-lubanu-s</t>
-  </si>
-  <si>
-    <t>10.921895980834961 s</t>
-  </si>
-  <si>
-    <t>O1CN01sCOsdn1iCFsxoq1hI_!!0-item_pic</t>
-  </si>
-  <si>
-    <t>10.922948837280273 s</t>
+    <t>13.57 s</t>
+  </si>
+  <si>
+    <t>O1CN01NVlKjz1GaFOADKpmu_!!738840638-0-lubanu-s.jpg_430x430q90</t>
+  </si>
+  <si>
+    <t>9.85 s</t>
+  </si>
+  <si>
+    <t>O1CN01sCOsdn1iCFsxoq1hI_!!0-item_pic.jpg_430x430q90</t>
+  </si>
+  <si>
+    <t>10.10 s</t>
   </si>
   <si>
     <t>Acrople-Jogger-Black-Front-View</t>
   </si>
   <si>
-    <t>70.87657904624939 s</t>
-  </si>
-  <si>
-    <t>O1CN01BrqcSl1nfdPrf5SSc_!!2111455117</t>
-  </si>
-  <si>
-    <t>8.119968891143799 s</t>
-  </si>
-  <si>
-    <t>O1CN0103BThs1bfqDmJGrAu_!!876583493</t>
-  </si>
-  <si>
-    <t>10.874741077423096 s</t>
-  </si>
-  <si>
-    <t>O1CN01xrQAtj1YAkUECeE7F_!!1695303019</t>
-  </si>
-  <si>
-    <t>9.77763295173645 s</t>
+    <t>78.30 s</t>
+  </si>
+  <si>
+    <t>O1CN01BrqcSl1nfdPrf5SSc_!!2111455117.jpg_430x430q90</t>
+  </si>
+  <si>
+    <t>8.53 s</t>
+  </si>
+  <si>
+    <t>O1CN0103BThs1bfqDmJGrAu_!!876583493.jpg_430x430q90</t>
+  </si>
+  <si>
+    <t>8.34 s</t>
+  </si>
+  <si>
+    <t>O1CN01xrQAtj1YAkUECeE7F_!!1695303019.jpg_430x430q90</t>
+  </si>
+  <si>
+    <t>8.65 s</t>
   </si>
   <si>
     <t>O1CN01qhJfFy1PJbVyiL4Tm_!!391751820</t>
   </si>
   <si>
-    <t>14.761693954467773 s</t>
+    <t>13.85 s</t>
   </si>
   <si>
     <t>O1CN01Q5o4xa1Iuyb8Z3URT_!!2421830954</t>
   </si>
   <si>
-    <t>png</t>
-  </si>
-  <si>
-    <t>37.82070589065552 s</t>
-  </si>
-  <si>
-    <t>O1CN01HvCSgF26eEuUNdZuX_!!0-item_pic</t>
-  </si>
-  <si>
-    <t>12.665625095367432 s</t>
-  </si>
-  <si>
-    <t>O1CN01yrU0f52CZ65hVx19M_!!0-item_pic</t>
-  </si>
-  <si>
-    <t>10.460567712783813 s</t>
+    <t>33.75 s</t>
+  </si>
+  <si>
+    <t>O1CN01HvCSgF26eEuUNdZuX_!!0-item_pic.jpg_430x430q90</t>
+  </si>
+  <si>
+    <t>9.92 s</t>
+  </si>
+  <si>
+    <t>O1CN01yrU0f52CZ65hVx19M_!!0-item_pic.jpg_430x430q90</t>
+  </si>
+  <si>
+    <t>11.10 s</t>
   </si>
   <si>
     <t>Beta-LT-Jacket-Hadron-Fluidity-Front-View</t>
   </si>
   <si>
-    <t>89.21676993370056 s</t>
+    <t>83.13 s</t>
   </si>
   <si>
     <t>d9fbad7d010f8d43</t>
   </si>
   <si>
-    <t>25.797447204589844 s</t>
+    <t>26.31 s</t>
   </si>
   <si>
     <t>Konseal-55-Backpack-Neptune-Back-View</t>
   </si>
   <si>
-    <t>76.82686710357666 s</t>
+    <t>72.39 s</t>
   </si>
   <si>
     <t>O1CN01ra3Zd31iCFsxoZmLa_!!733534376</t>
   </si>
   <si>
-    <t>49.979650259017944 s</t>
+    <t>43.56 s</t>
   </si>
   <si>
     <t>O1CN01tJMOUo1rLG7FFPzQS_!!181395614</t>
   </si>
   <si>
-    <t>25.050055742263794 s</t>
+    <t>23.65 s</t>
   </si>
   <si>
     <t>2faa6023-1af9-4135-8dfc-8577ab09e37c</t>
   </si>
   <si>
-    <t>17.255316972732544 s</t>
+    <t>15.71 s</t>
   </si>
   <si>
     <t>O1CN01eAxs8z2KGnFJM1Oo3_!!856169530</t>
   </si>
   <si>
-    <t>134.56233596801758 s</t>
+    <t>133.36 s</t>
   </si>
   <si>
     <t>cc307_b4rh5_a0</t>
   </si>
   <si>
-    <t>84.12614893913269 s</t>
-  </si>
-  <si>
-    <t>O1CN01joq6MU1eG8pyNoSyY_!!3697853843</t>
-  </si>
-  <si>
-    <t>9.185529232025146 s</t>
+    <t>74.93 s</t>
+  </si>
+  <si>
+    <t>O1CN01joq6MU1eG8pyNoSyY_!!3697853843.jpg_430x430q90</t>
+  </si>
+  <si>
+    <t>8.25 s</t>
   </si>
   <si>
     <t>ca127_b4iy_a0</t>
   </si>
   <si>
-    <t>84.14233922958374 s</t>
-  </si>
-  <si>
-    <t>O1CN01jP86rN1QpUcyWOcTx_!!1909132025</t>
-  </si>
-  <si>
-    <t>9.881677150726318 s</t>
+    <t>79.29 s</t>
+  </si>
+  <si>
+    <t>O1CN01jP86rN1QpUcyWOcTx_!!1909132025.jpg_430x430q90</t>
+  </si>
+  <si>
+    <t>10.67 s</t>
   </si>
   <si>
     <t>xeric-vendetta-wandering-hour-automatic-5_720x</t>
   </si>
   <si>
-    <t>23.88613510131836 s</t>
-  </si>
-  <si>
-    <t>O1CN0103avRu1LHzkaUFMYb_!!0-item_pic</t>
-  </si>
-  <si>
-    <t>11.151971101760864 s</t>
+    <t>19.13 s</t>
+  </si>
+  <si>
+    <t>O1CN0103avRu1LHzkaUFMYb_!!0-item_pic.jpg_430x430q90</t>
+  </si>
+  <si>
+    <t>11.03 s</t>
   </si>
   <si>
     <t>D-CONVERSE-06-16-22-GBL-HP-BACKUP-MARBLED-1</t>
   </si>
   <si>
-    <t>48.53830909729004 s</t>
+    <t>44.34 s</t>
   </si>
   <si>
     <t>O1CN01pGzOYj1yAucFrBlZb_!!664396539</t>
   </si>
   <si>
-    <t>29.85483407974243 s</t>
+    <t>31.11 s</t>
   </si>
   <si>
     <t>Contenta-Dress-Melange-Atmos-Heather-Women-s-Front-View</t>
   </si>
   <si>
-    <t>80.3816032409668 s</t>
-  </si>
-  <si>
-    <t>O1CN019NcSGW2NUwFnzs79L_!!729289967</t>
-  </si>
-  <si>
-    <t>11.298235893249512 s</t>
+    <t>76.34 s</t>
+  </si>
+  <si>
+    <t>O1CN019NcSGW2NUwFnzs79L_!!729289967.jpg_430x430q90</t>
+  </si>
+  <si>
+    <t>9.41 s</t>
   </si>
   <si>
     <t>O1CN01pcSF4r1UQ5Gz4GDVi_!!2211935182511</t>
   </si>
   <si>
-    <t>22.576110124588013 s</t>
+    <t>25.16 s</t>
   </si>
   <si>
     <t>799153b0-1715-425f-b672-7bd6926680ff</t>
   </si>
   <si>
-    <t>14.982159852981567 s</t>
-  </si>
-  <si>
-    <t>O1CN01uMDed51sYpSyH3cHI_!!1813135779</t>
-  </si>
-  <si>
-    <t>11.147072076797485 s</t>
+    <t>11.51 s</t>
+  </si>
+  <si>
+    <t>O1CN01uMDed51sYpSyH3cHI_!!1813135779.jpg_430x430q90</t>
+  </si>
+  <si>
+    <t>8.92 s</t>
   </si>
   <si>
     <t>总时间：</t>
   </si>
   <si>
-    <t>1493.7944600582123 s</t>
+    <t>1444.83 s</t>
   </si>
   <si>
     <t>平均时间：</t>
   </si>
   <si>
-    <t>31.782860852302388 s</t>
+    <t>30.74 s</t>
   </si>
 </sst>
 </file>
@@ -714,10 +708,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -725,13 +719,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -739,13 +733,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -753,13 +747,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -767,13 +761,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -781,13 +775,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -795,13 +789,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -809,13 +803,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -823,13 +817,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -837,13 +831,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -851,13 +845,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
         <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -865,13 +859,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
         <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -879,13 +873,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
         <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -893,13 +887,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
         <v>36</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -907,13 +901,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
         <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -921,13 +915,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
         <v>40</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -935,13 +929,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
         <v>42</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -949,13 +943,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
         <v>44</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -963,13 +957,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
         <v>46</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -977,13 +971,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
         <v>48</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -991,13 +985,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
         <v>50</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1005,13 +999,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
         <v>52</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1019,13 +1013,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
         <v>54</v>
-      </c>
-      <c r="C25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1033,13 +1027,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
         <v>56</v>
-      </c>
-      <c r="C26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1047,13 +1041,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1061,13 +1055,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1075,13 +1069,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1089,13 +1083,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1103,13 +1097,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1117,13 +1111,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1131,13 +1125,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1145,13 +1139,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1159,13 +1153,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1173,13 +1167,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1187,13 +1181,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1201,13 +1195,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1215,13 +1209,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1229,13 +1223,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1243,13 +1237,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1257,13 +1251,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1271,13 +1265,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1285,13 +1279,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1299,13 +1293,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1313,13 +1307,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1327,13 +1321,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1341,29 +1335,29 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="3:4">
       <c r="C49" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D49" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="3:4">
       <c r="C50" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D50" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>